<commit_message>
finished main.py started plot.py
</commit_message>
<xml_diff>
--- a/Biesktion_PHinterbauer.xlsx
+++ b/Biesktion_PHinterbauer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tgmwien-my.sharepoint.com/personal/phinterbauer_student_tgm_ac_at/Documents/TGM_Hinterbauer/SWP/3BHWII/Bisektion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="8_{F3DE3F44-59AD-44D8-A346-8E446DD3BAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4566B1C-5984-409A-93B7-CE07AD9DEE5B}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="8_{F3DE3F44-59AD-44D8-A346-8E446DD3BAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C89FB4D7-FC71-465C-B450-2C8508BCE7D6}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{597A8E95-AD4D-4137-864C-7E939DD9B357}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>a</t>
   </si>
@@ -63,12 +63,6 @@
   </si>
   <si>
     <t>Iter</t>
-  </si>
-  <si>
-    <t>f(a) * f(b) &lt; 1</t>
-  </si>
-  <si>
-    <t>f(a) * f(b) &lt; 2</t>
   </si>
 </sst>
 </file>
@@ -123,7 +117,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -132,19 +126,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -3524,9 +3511,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E9F9376-0247-4E0F-8C71-760424359805}" name="Tabelle1" displayName="Tabelle1" ref="A10:J21" totalsRowShown="0">
-  <autoFilter ref="A10:J21" xr:uid="{9E9F9376-0247-4E0F-8C71-760424359805}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E9F9376-0247-4E0F-8C71-760424359805}" name="Tabelle1" displayName="Tabelle1" ref="A10:H21" totalsRowShown="0">
+  <autoFilter ref="A10:H21" xr:uid="{9E9F9376-0247-4E0F-8C71-760424359805}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{9E10774E-B7E3-4412-B384-E7FB447919AE}" name="Iter"/>
     <tableColumn id="2" xr3:uid="{3BDAFD8F-DBEF-44E2-8256-E93CED69D20F}" name="a">
       <calculatedColumnFormula>IF(G10 &lt; 0, B10, F10)</calculatedColumnFormula>
@@ -3534,26 +3521,20 @@
     <tableColumn id="3" xr3:uid="{711539B0-7A38-420B-A2ED-7269AF4AF14C}" name="b">
       <calculatedColumnFormula>IF(G10 &gt; 0,C10,F10)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{41584A57-D715-403B-8FBD-650A8C4DEF21}" name="f(a)" dataDxfId="15">
+    <tableColumn id="4" xr3:uid="{41584A57-D715-403B-8FBD-650A8C4DEF21}" name="f(a)" dataDxfId="13">
       <calculatedColumnFormula>SQRT(28) - B11</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C366ED33-5181-4E71-A176-F0DC5439C9C2}" name="f(b)" dataDxfId="14">
+    <tableColumn id="5" xr3:uid="{C366ED33-5181-4E71-A176-F0DC5439C9C2}" name="f(b)" dataDxfId="12">
       <calculatedColumnFormula>SQRT(28) - C11</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{C448E66C-7B89-4FF8-823E-401A1212745D}" name="c">
       <calculatedColumnFormula>(B11+C11)/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{209B61C3-49DC-4EC4-8ED8-6533389D83C2}" name="f(c) " dataDxfId="13">
+    <tableColumn id="7" xr3:uid="{209B61C3-49DC-4EC4-8ED8-6533389D83C2}" name="f(c) " dataDxfId="11">
       <calculatedColumnFormula>SQRT(28) - F11</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{76B31415-6376-40FA-8FB4-F2924A32E937}" name="f(a) * f(b) &lt; 0">
       <calculatedColumnFormula>D11*E11</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{B6954842-5CA2-45C6-A95B-A24EA5BF3F5B}" name="f(a) * f(b) &lt; 1" dataDxfId="1">
-      <calculatedColumnFormula>IF((Tabelle1[[#This Row],[f(a)]]*Tabelle1[[#This Row],[f(c) ]])&gt;0, Tabelle1[[#This Row],[b]],Tabelle1[[#This Row],[a]])</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="10" xr3:uid="{32B8F274-5ECC-4389-983D-1FD9950A7397}" name="f(a) * f(b) &lt; 2" dataDxfId="0">
-      <calculatedColumnFormula>IF(ABS(Tabelle1[[#This Row],[f(c) ]])&gt;0.001,FALSE,TRUE)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3567,16 +3548,16 @@
     <tableColumn id="1" xr3:uid="{2A2CB383-CD53-401D-94CF-7832F1474B2B}" name="Iter"/>
     <tableColumn id="2" xr3:uid="{44DDA779-8B62-4518-8E03-EE4BB834E3DC}" name="a"/>
     <tableColumn id="3" xr3:uid="{4D2C07A3-10E4-4D7D-B6AE-1862469A47F1}" name="b"/>
-    <tableColumn id="4" xr3:uid="{6158B74D-35EE-40E7-9A39-CB061EA6AF28}" name="f(a)" dataDxfId="12">
+    <tableColumn id="4" xr3:uid="{6158B74D-35EE-40E7-9A39-CB061EA6AF28}" name="f(a)" dataDxfId="10">
       <calculatedColumnFormula>SQRT(6) - B35</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F76587D5-36B9-4B32-A157-2128CD39363A}" name="f(b)" dataDxfId="11">
+    <tableColumn id="5" xr3:uid="{F76587D5-36B9-4B32-A157-2128CD39363A}" name="f(b)" dataDxfId="9">
       <calculatedColumnFormula>SQRT(6) - C35</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{36C872E6-07C0-491D-A57B-DD2F55C6E350}" name="c">
       <calculatedColumnFormula>(B35+C35)/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E7159FD2-DD6B-48AB-B957-600049027CB0}" name="f(c) " dataDxfId="10">
+    <tableColumn id="7" xr3:uid="{E7159FD2-DD6B-48AB-B957-600049027CB0}" name="f(c) " dataDxfId="8">
       <calculatedColumnFormula>SQRT(6) - F35</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{EA5095EA-FB82-4D87-860D-5DE99CDAF703}" name="f(a) * f(b) &lt; 0">
@@ -3907,9 +3888,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -3920,7 +3901,7 @@
     <col min="8" max="8" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -3930,7 +3911,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -3940,7 +3921,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3950,7 +3931,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -3960,7 +3941,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -3970,7 +3951,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -3980,7 +3961,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -3990,7 +3971,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -4000,7 +3981,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -4010,7 +3991,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -4035,14 +4016,8 @@
       <c r="H10" t="s">
         <v>6</v>
       </c>
-      <c r="I10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -4072,16 +4047,8 @@
         <f t="shared" ref="H11:H16" si="2">D11*E11</f>
         <v>-120.16207341961709</v>
       </c>
-      <c r="I11" s="4">
-        <f>IF((Tabelle1[[#This Row],[f(a)]]*Tabelle1[[#This Row],[f(c) ]])&gt;0, Tabelle1[[#This Row],[b]],Tabelle1[[#This Row],[a]])</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="4" t="b">
-        <f>IF(ABS(Tabelle1[[#This Row],[f(c) ]])&gt;0.001,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -4113,16 +4080,8 @@
         <f t="shared" si="2"/>
         <v>-46.081036709808537</v>
       </c>
-      <c r="I12" s="4">
-        <f>IF((Tabelle1[[#This Row],[f(a)]]*Tabelle1[[#This Row],[f(c) ]])&gt;0, Tabelle1[[#This Row],[b]],Tabelle1[[#This Row],[a]])</f>
-        <v>0</v>
-      </c>
-      <c r="J12" s="4" t="b">
-        <f>IF(ABS(Tabelle1[[#This Row],[f(c) ]])&gt;0.001,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -4154,16 +4113,8 @@
         <f t="shared" si="2"/>
         <v>-9.0405183549042683</v>
       </c>
-      <c r="I13" s="4">
-        <f>IF((Tabelle1[[#This Row],[f(a)]]*Tabelle1[[#This Row],[f(c) ]])&gt;0, Tabelle1[[#This Row],[b]],Tabelle1[[#This Row],[a]])</f>
-        <v>7</v>
-      </c>
-      <c r="J13" s="4" t="b">
-        <f>IF(ABS(Tabelle1[[#This Row],[f(c) ]])&gt;0.001,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4</v>
       </c>
@@ -4195,16 +4146,8 @@
         <f t="shared" si="2"/>
         <v>-3.0607775323564024</v>
       </c>
-      <c r="I14" s="4">
-        <f>IF((Tabelle1[[#This Row],[f(a)]]*Tabelle1[[#This Row],[f(c) ]])&gt;0, Tabelle1[[#This Row],[b]],Tabelle1[[#This Row],[a]])</f>
-        <v>7</v>
-      </c>
-      <c r="J14" s="4" t="b">
-        <f>IF(ABS(Tabelle1[[#This Row],[f(c) ]])&gt;0.001,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5</v>
       </c>
@@ -4236,16 +4179,8 @@
         <f t="shared" si="2"/>
         <v>-7.0907121082469882E-2</v>
       </c>
-      <c r="I15" s="4">
-        <f>IF((Tabelle1[[#This Row],[f(a)]]*Tabelle1[[#This Row],[f(c) ]])&gt;0, Tabelle1[[#This Row],[b]],Tabelle1[[#This Row],[a]])</f>
-        <v>5.25</v>
-      </c>
-      <c r="J15" s="4" t="b">
-        <f>IF(ABS(Tabelle1[[#This Row],[f(c) ]])&gt;0.001,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>6</v>
       </c>
@@ -4277,16 +4212,8 @@
         <f t="shared" si="2"/>
         <v>-3.4592326719436135E-2</v>
       </c>
-      <c r="I16" s="4">
-        <f>IF((Tabelle1[[#This Row],[f(a)]]*Tabelle1[[#This Row],[f(c) ]])&gt;0, Tabelle1[[#This Row],[b]],Tabelle1[[#This Row],[a]])</f>
-        <v>5.25</v>
-      </c>
-      <c r="J16" s="4" t="b">
-        <f>IF(ABS(Tabelle1[[#This Row],[f(c) ]])&gt;0.001,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>7</v>
       </c>
@@ -4318,16 +4245,8 @@
         <f t="shared" ref="H17:H18" si="8">D17*E17</f>
         <v>-1.6434929537919255E-2</v>
       </c>
-      <c r="I17" s="4">
-        <f>IF((Tabelle1[[#This Row],[f(a)]]*Tabelle1[[#This Row],[f(c) ]])&gt;0, Tabelle1[[#This Row],[b]],Tabelle1[[#This Row],[a]])</f>
-        <v>5.25</v>
-      </c>
-      <c r="J17" s="4" t="b">
-        <f>IF(ABS(Tabelle1[[#This Row],[f(c) ]])&gt;0.001,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>8</v>
       </c>
@@ -4359,16 +4278,8 @@
         <f t="shared" si="8"/>
         <v>-7.3562309471608177E-3</v>
       </c>
-      <c r="I18" s="4">
-        <f>IF((Tabelle1[[#This Row],[f(a)]]*Tabelle1[[#This Row],[f(c) ]])&gt;0, Tabelle1[[#This Row],[b]],Tabelle1[[#This Row],[a]])</f>
-        <v>5.25</v>
-      </c>
-      <c r="J18" s="4" t="b">
-        <f>IF(ABS(Tabelle1[[#This Row],[f(c) ]])&gt;0.001,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>9</v>
       </c>
@@ -4397,19 +4308,11 @@
         <v>-1.3184877870818568E-2</v>
       </c>
       <c r="H19">
-        <f t="shared" ref="H19:H21" si="15">D19*E19</f>
+        <f t="shared" ref="H19:H20" si="15">D19*E19</f>
         <v>-2.816881651781599E-3</v>
       </c>
-      <c r="I19" s="4">
-        <f>IF((Tabelle1[[#This Row],[f(a)]]*Tabelle1[[#This Row],[f(c) ]])&gt;0, Tabelle1[[#This Row],[b]],Tabelle1[[#This Row],[a]])</f>
-        <v>5.25</v>
-      </c>
-      <c r="J19" s="4" t="b">
-        <f>IF(ABS(Tabelle1[[#This Row],[f(c) ]])&gt;0.001,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10</v>
       </c>
@@ -4441,16 +4344,8 @@
         <f t="shared" si="15"/>
         <v>-5.472070040919893E-4</v>
       </c>
-      <c r="I20" s="4">
-        <f>IF((Tabelle1[[#This Row],[f(a)]]*Tabelle1[[#This Row],[f(c) ]])&gt;0, Tabelle1[[#This Row],[b]],Tabelle1[[#This Row],[a]])</f>
-        <v>5.3046875</v>
-      </c>
-      <c r="J20" s="4" t="b">
-        <f>IF(ABS(Tabelle1[[#This Row],[f(c) ]])&gt;0.001,FALSE,TRUE)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>11</v>
       </c>
@@ -4482,16 +4377,8 @@
         <f>D21*E21</f>
         <v>-1.8668299981179404E-4</v>
       </c>
-      <c r="I21" s="4">
-        <f>IF((Tabelle1[[#This Row],[f(a)]]*Tabelle1[[#This Row],[f(c) ]])&gt;0, Tabelle1[[#This Row],[b]],Tabelle1[[#This Row],[a]])</f>
-        <v>5.3046875</v>
-      </c>
-      <c r="J21" s="4" t="b">
-        <f>IF(ABS(Tabelle1[[#This Row],[f(c) ]])&gt;0.001,FALSE,TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -4501,7 +4388,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -4511,7 +4398,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -4521,7 +4408,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -4531,7 +4418,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -4541,7 +4428,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -4551,7 +4438,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -4561,7 +4448,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -4571,7 +4458,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -4581,7 +4468,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -4591,7 +4478,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -4932,34 +4819,34 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B11:B21 B35:B38">
-    <cfRule type="expression" dxfId="9" priority="11">
+    <cfRule type="expression" dxfId="7" priority="11">
       <formula>G11 &lt; 0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="12">
+    <cfRule type="expression" dxfId="6" priority="12">
       <formula>G11 &gt;= 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C20 C35:C39">
-    <cfRule type="expression" dxfId="7" priority="9">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>G11 &lt; 0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="10">
+    <cfRule type="expression" dxfId="4" priority="10">
       <formula>G11 &gt;= 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11:H21">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>H11 &gt;= 0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>H11 &lt; 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35:H39">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>H35 &gt;= 0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>H35 &lt; 0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>